<commit_message>
Complete the seond iteration of the project.
</commit_message>
<xml_diff>
--- a/custom/attendance_sheet.xlsx
+++ b/custom/attendance_sheet.xlsx
@@ -440,17 +440,17 @@
           <t>QA</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="0" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="0" t="inlineStr">
         <is>
           <t>Answered</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="0" t="inlineStr">
         <is>
           <t>QA</t>
         </is>
@@ -469,22 +469,62 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>2021-11-11</t>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>1, 2</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>2021-11-11</t>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>2021-11-11</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2021-11-11</t>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>1, 2</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -501,22 +541,52 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-11</t>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-11</t>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>2, 3</t>
+        </is>
+      </c>
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-11</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>2021-11-11</t>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="M3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a function to automate scheduling.
</commit_message>
<xml_diff>
--- a/custom/attendance_sheet.xlsx
+++ b/custom/attendance_sheet.xlsx
@@ -376,7 +376,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:BV3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,306 @@
           <t>QA</t>
         </is>
       </c>
+      <c r="O1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="P1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="R1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="S1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="T1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="U1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="V1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="W1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="X1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="Y1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="Z1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AA1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AB1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AC1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AD1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AE1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AF1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AG1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AH1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AI1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AJ1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AK1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AL1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AM1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AN1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AO1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AP1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AQ1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AR1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AS1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AT1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AU1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AV1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AW1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="AX1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="AY1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="AZ1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BA1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BB1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BC1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BD1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BE1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BF1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BG1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BH1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BI1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BJ1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BK1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BL1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BM1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BN1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BO1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BP1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BQ1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BR1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BS1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="BT1" s="0" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="BU1" s="0" t="inlineStr">
+        <is>
+          <t>Answered</t>
+        </is>
+      </c>
+      <c r="BV1" s="0" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -469,60 +769,230 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="L2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="O2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="Q2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="T2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="W2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="Z2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AC2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AF2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AI2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AJ2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AL2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AM2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AO2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AR2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AS2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AU2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AV2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AX2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AY2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BA2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BB2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BD2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BE2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BG2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BH2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BJ2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BK2" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BM2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BN2" s="0" t="inlineStr">
+        <is>
+          <t>Fri Dec. 3/2021</t>
+        </is>
+      </c>
+      <c r="BO2" s="0" t="inlineStr">
         <is>
           <t>1, 2</t>
         </is>
       </c>
-      <c r="E2" s="0" t="inlineStr">
+      <c r="BP2" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="F2" s="0" t="inlineStr">
-        <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="G2" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H2" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" s="0" t="inlineStr">
-        <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="J2" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K2" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L2" s="0" t="inlineStr">
-        <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="M2" s="0" t="inlineStr">
+      <c r="BQ2" s="0" t="inlineStr">
+        <is>
+          <t>Wed Dec. 22/2021</t>
+        </is>
+      </c>
+      <c r="BS2" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BT2" s="0" t="inlineStr">
+        <is>
+          <t>Wed Dec. 22/2021</t>
+        </is>
+      </c>
+      <c r="BU2" s="0" t="inlineStr">
         <is>
           <t>1, 2</t>
         </is>
       </c>
-      <c r="N2" s="0" t="inlineStr">
+      <c r="BV2" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -541,52 +1011,222 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>2021-11-11</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="G3" s="0" t="inlineStr">
-        <is>
-          <t>2, 3</t>
-        </is>
-      </c>
-      <c r="H3" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>2021-11-11</t>
         </is>
       </c>
       <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="K3" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>2021-11-11</t>
         </is>
       </c>
       <c r="L3" s="0" t="inlineStr">
         <is>
-          <t>2021-11-12</t>
-        </is>
-      </c>
-      <c r="M3" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="N3" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>2021-11-11</t>
+        </is>
+      </c>
+      <c r="O3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="Q3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="T3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="W3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="Z3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AC3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AF3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AI3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AJ3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AL3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AM3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AO3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AR3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AS3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AU3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AV3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="AX3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AY3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BA3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BB3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BD3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BE3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BG3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BH3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BJ3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BK3" s="0" t="inlineStr">
+        <is>
+          <t>2021-11-12</t>
+        </is>
+      </c>
+      <c r="BM3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BN3" s="0" t="inlineStr">
+        <is>
+          <t>Fri Dec. 3/2021</t>
+        </is>
+      </c>
+      <c r="BP3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BQ3" s="0" t="inlineStr">
+        <is>
+          <t>Wed Dec. 22/2021</t>
+        </is>
+      </c>
+      <c r="BS3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BT3" s="0" t="inlineStr">
+        <is>
+          <t>Wed Dec. 22/2021</t>
+        </is>
+      </c>
+      <c r="BV3" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>